<commit_message>
Send message to single user added
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PetrK\Desktop\Projects\Notification-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABCF91D-458C-458C-B76D-FBAED8FCF736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D3DE00-2861-4101-A586-686A91B58175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF8E12E7-B21F-4C78-A91B-2E37E214AFD5}"/>
   </bookViews>
@@ -44,10 +44,10 @@
     <t>ITS me</t>
   </si>
   <si>
-    <t>111-222111-11</t>
+    <t>capin19887@kernuo.com</t>
   </si>
   <si>
-    <t>pitayo6075@fna6.com</t>
+    <t>komajox883@fna6.com</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +445,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -453,7 +453,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kafka commiting added + Random selection of partition
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PetrK\Desktop\Projects\Notification-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D3DE00-2861-4101-A586-686A91B58175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA8C519-9EFF-4BAD-8428-DF198E845D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF8E12E7-B21F-4C78-A91B-2E37E214AFD5}"/>
   </bookViews>
@@ -38,16 +38,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>testPerson2</t>
+    <t>komajox883@fna6.com</t>
   </si>
   <si>
-    <t>ITS me</t>
+    <t>FirstUser</t>
   </si>
   <si>
-    <t>capin19887@kernuo.com</t>
+    <t>SecondUSer</t>
   </si>
   <si>
-    <t>komajox883@fna6.com</t>
+    <t>layidak603@morxin.com</t>
   </si>
 </sst>
 </file>
@@ -445,12 +445,12 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Unic name in contacts file added
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PetrK\Desktop\Projects\Notification-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA8C519-9EFF-4BAD-8428-DF198E845D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1889A2B-A7A6-42D3-B97C-9EB08F9B1280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF8E12E7-B21F-4C78-A91B-2E37E214AFD5}"/>
   </bookViews>
@@ -36,18 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>komajox883@fna6.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>FirstUser</t>
   </si>
   <si>
-    <t>SecondUSer</t>
+    <t>aa@mail.com</t>
   </si>
   <si>
-    <t>layidak603@morxin.com</t>
+    <t>asd@Gmail.com</t>
   </si>
 </sst>
 </file>
@@ -442,21 +439,25 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{1D154A37-8CD4-4DDC-BC39-B4FEF884FBC0}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{45D474E2-EA91-4CDE-92A7-3FF932E020DC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>